<commit_message>
change nested loop to if gen and replace if(xy[i]) o +=xy[i] in hamming.v
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="501" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="151" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -165,7 +165,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -197,8 +197,8 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R9" activeCellId="0" sqref="R9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V6" activeCellId="0" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -364,25 +364,25 @@
         <v>7888</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>834</v>
+        <v>496</v>
       </c>
       <c r="Q5" s="0" t="n">
-        <v>1095</v>
+        <v>332</v>
       </c>
       <c r="R5" s="0" t="n">
         <f aca="false">SUM(P5:Q5)</f>
-        <v>1929</v>
+        <v>828</v>
       </c>
       <c r="S5" s="0" t="n">
-        <v>1357</v>
+        <v>486</v>
       </c>
       <c r="T5" s="0" t="n">
         <f aca="false">SUM(P5:R5)</f>
-        <v>3858</v>
+        <v>1656</v>
       </c>
       <c r="U5" s="1" t="n">
         <f aca="false">SUM(P5:Q5)+5*S5</f>
-        <v>8714</v>
+        <v>3258</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -428,25 +428,25 @@
         <v>58412</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>12780</v>
+        <v>4825</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <v>18603</v>
+        <v>3126</v>
       </c>
       <c r="R6" s="0" t="n">
         <f aca="false">SUM(P6:Q6)</f>
-        <v>31383</v>
+        <v>7951</v>
       </c>
       <c r="S6" s="0" t="n">
-        <v>22718</v>
+        <v>4810</v>
       </c>
       <c r="T6" s="0" t="n">
         <f aca="false">SUM(P6:R6)</f>
-        <v>62766</v>
+        <v>15902</v>
       </c>
       <c r="U6" s="1" t="n">
         <f aca="false">SUM(P6:Q6)+5*S6</f>
-        <v>144973</v>
+        <v>32001</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add alu result and change lib for xor from 1000 to 5
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Function</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Mult</t>
+  </si>
+  <si>
+    <t>alu</t>
   </si>
 </sst>
 </file>
@@ -195,10 +198,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V6" activeCellId="0" sqref="V6"/>
+      <selection pane="topLeft" activeCell="U20" activeCellId="0" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -786,6 +789,64 @@
         <v>390730</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <f aca="false">SUM(P15:Q15)</f>
+        <v>107</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <f aca="false">SUM(P15:R15)</f>
+        <v>214</v>
+      </c>
+      <c r="U15" s="1" t="n">
+        <f aca="false">SUM(P15:Q15)+5*S15</f>
+        <v>922</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <f aca="false">SUM(P16:Q16)</f>
+        <v>359</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <v>422</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <f aca="false">SUM(P16:R16)</f>
+        <v>718</v>
+      </c>
+      <c r="U16" s="1" t="n">
+        <f aca="false">SUM(P16:Q16)+5*S16</f>
+        <v>2469</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:I1"/>

</xml_diff>

<commit_message>
add synthesized alu with abc and update results
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="151" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="76" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -200,8 +200,8 @@
   </sheetPr>
   <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U20" activeCellId="0" sqref="U20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S25" activeCellId="0" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -366,24 +366,24 @@
         <f aca="false">K5+(L5*5)</f>
         <v>7888</v>
       </c>
-      <c r="P5" s="0" t="n">
+      <c r="P5" s="7" t="n">
         <v>496</v>
       </c>
-      <c r="Q5" s="0" t="n">
+      <c r="Q5" s="7" t="n">
         <v>332</v>
       </c>
-      <c r="R5" s="0" t="n">
+      <c r="R5" s="7" t="n">
         <f aca="false">SUM(P5:Q5)</f>
         <v>828</v>
       </c>
-      <c r="S5" s="0" t="n">
+      <c r="S5" s="7" t="n">
         <v>486</v>
       </c>
-      <c r="T5" s="0" t="n">
+      <c r="T5" s="7" t="n">
         <f aca="false">SUM(P5:R5)</f>
         <v>1656</v>
       </c>
-      <c r="U5" s="1" t="n">
+      <c r="U5" s="6" t="n">
         <f aca="false">SUM(P5:Q5)+5*S5</f>
         <v>3258</v>
       </c>
@@ -430,24 +430,24 @@
         <f aca="false">K6+(L6*5)</f>
         <v>58412</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="P6" s="7" t="n">
         <v>4825</v>
       </c>
-      <c r="Q6" s="0" t="n">
+      <c r="Q6" s="7" t="n">
         <v>3126</v>
       </c>
-      <c r="R6" s="0" t="n">
+      <c r="R6" s="7" t="n">
         <f aca="false">SUM(P6:Q6)</f>
         <v>7951</v>
       </c>
-      <c r="S6" s="0" t="n">
+      <c r="S6" s="7" t="n">
         <v>4810</v>
       </c>
-      <c r="T6" s="0" t="n">
+      <c r="T6" s="7" t="n">
         <f aca="false">SUM(P6:R6)</f>
         <v>15902</v>
       </c>
-      <c r="U6" s="1" t="n">
+      <c r="U6" s="6" t="n">
         <f aca="false">SUM(P6:Q6)+5*S6</f>
         <v>32001</v>
       </c>
@@ -467,7 +467,12 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="6"/>
-      <c r="U7" s="1"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -513,24 +518,24 @@
         <f aca="false">K8+(L8*5)</f>
         <v>2823</v>
       </c>
-      <c r="P8" s="0" t="n">
+      <c r="P8" s="7" t="n">
         <v>370</v>
       </c>
-      <c r="Q8" s="0" t="n">
+      <c r="Q8" s="7" t="n">
         <v>486</v>
       </c>
-      <c r="R8" s="0" t="n">
+      <c r="R8" s="7" t="n">
         <f aca="false">SUM(P8:Q8)</f>
         <v>856</v>
       </c>
-      <c r="S8" s="0" t="n">
+      <c r="S8" s="7" t="n">
         <v>384</v>
       </c>
-      <c r="T8" s="0" t="n">
+      <c r="T8" s="7" t="n">
         <f aca="false">SUM(P8:R8)</f>
         <v>1712</v>
       </c>
-      <c r="U8" s="1" t="n">
+      <c r="U8" s="6" t="n">
         <f aca="false">SUM(P8:Q8)+5*S8</f>
         <v>2776</v>
       </c>
@@ -577,24 +582,24 @@
         <f aca="false">K9+(L9*5)</f>
         <v>5835</v>
       </c>
-      <c r="P9" s="0" t="n">
+      <c r="P9" s="7" t="n">
         <v>756</v>
       </c>
-      <c r="Q9" s="0" t="n">
+      <c r="Q9" s="7" t="n">
         <v>1002</v>
       </c>
-      <c r="R9" s="0" t="n">
+      <c r="R9" s="7" t="n">
         <f aca="false">SUM(P9:Q9)</f>
         <v>1758</v>
       </c>
-      <c r="S9" s="0" t="n">
+      <c r="S9" s="7" t="n">
         <v>768</v>
       </c>
-      <c r="T9" s="0" t="n">
+      <c r="T9" s="7" t="n">
         <f aca="false">SUM(P9:R9)</f>
         <v>3516</v>
       </c>
-      <c r="U9" s="1" t="n">
+      <c r="U9" s="6" t="n">
         <f aca="false">SUM(P9:Q9)+5*S9</f>
         <v>5598</v>
       </c>
@@ -641,7 +646,12 @@
         <f aca="false">K10+(L10*5)</f>
         <v>23907</v>
       </c>
-      <c r="U10" s="1"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
@@ -658,7 +668,12 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="6"/>
-      <c r="U11" s="1"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -704,29 +719,30 @@
         <f aca="false">K12+(L12*5)</f>
         <v>204944</v>
       </c>
-      <c r="P12" s="0" t="n">
+      <c r="P12" s="7" t="n">
         <v>8028</v>
       </c>
-      <c r="Q12" s="0" t="n">
+      <c r="Q12" s="7" t="n">
         <v>7337</v>
       </c>
-      <c r="R12" s="0" t="n">
+      <c r="R12" s="7" t="n">
         <f aca="false">SUM(P12:Q12)</f>
         <v>15365</v>
       </c>
-      <c r="S12" s="0" t="n">
+      <c r="S12" s="7" t="n">
         <v>16593</v>
       </c>
-      <c r="T12" s="0" t="n">
+      <c r="T12" s="7" t="n">
         <f aca="false">SUM(P12:R12)</f>
         <v>30730</v>
       </c>
-      <c r="U12" s="1" t="n">
+      <c r="U12" s="6" t="n">
         <f aca="false">SUM(P12:Q12)+5*S12</f>
         <v>98330</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
       <c r="B13" s="6" t="n">
         <v>128</v>
       </c>
@@ -767,30 +783,40 @@
         <f aca="false">K13+(L13*5)</f>
         <v>824064</v>
       </c>
-      <c r="P13" s="0" t="n">
+      <c r="P13" s="7" t="n">
         <v>32489</v>
       </c>
-      <c r="Q13" s="0" t="n">
+      <c r="Q13" s="7" t="n">
         <v>27891</v>
       </c>
-      <c r="R13" s="0" t="n">
+      <c r="R13" s="7" t="n">
         <f aca="false">SUM(P13:Q13)</f>
         <v>60380</v>
       </c>
-      <c r="S13" s="0" t="n">
+      <c r="S13" s="7" t="n">
         <v>66070</v>
       </c>
-      <c r="T13" s="0" t="n">
+      <c r="T13" s="7" t="n">
         <f aca="false">SUM(P13:R13)</f>
         <v>120760</v>
       </c>
-      <c r="U13" s="1" t="n">
+      <c r="U13" s="6" t="n">
         <f aca="false">SUM(P13:Q13)+5*S13</f>
         <v>390730</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="U14" s="1"/>
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+      <c r="F14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -799,24 +825,45 @@
       <c r="B15" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="P15" s="0" t="n">
+      <c r="D15" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <f aca="false">D15+E15</f>
+        <v>152</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <f aca="false">D15+E15+G15</f>
+        <v>347</v>
+      </c>
+      <c r="I15" s="6" t="n">
+        <f aca="false">F15+(G15*5)</f>
+        <v>1127</v>
+      </c>
+      <c r="P15" s="7" t="n">
         <v>26</v>
       </c>
-      <c r="Q15" s="0" t="n">
+      <c r="Q15" s="7" t="n">
         <v>81</v>
       </c>
-      <c r="R15" s="0" t="n">
+      <c r="R15" s="7" t="n">
         <f aca="false">SUM(P15:Q15)</f>
         <v>107</v>
       </c>
-      <c r="S15" s="0" t="n">
+      <c r="S15" s="7" t="n">
         <v>163</v>
       </c>
-      <c r="T15" s="0" t="n">
+      <c r="T15" s="7" t="n">
         <f aca="false">SUM(P15:R15)</f>
         <v>214</v>
       </c>
-      <c r="U15" s="1" t="n">
+      <c r="U15" s="6" t="n">
         <f aca="false">SUM(P15:Q15)+5*S15</f>
         <v>922</v>
       </c>
@@ -825,24 +872,45 @@
       <c r="B16" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="P16" s="0" t="n">
+      <c r="D16" s="0" t="n">
+        <v>211</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>346</v>
+      </c>
+      <c r="F16" s="7" t="n">
+        <f aca="false">D16+E16</f>
+        <v>557</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>685</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <f aca="false">D16+E16+G16</f>
+        <v>1242</v>
+      </c>
+      <c r="I16" s="6" t="n">
+        <f aca="false">F16+(G16*5)</f>
+        <v>3982</v>
+      </c>
+      <c r="P16" s="7" t="n">
         <v>139</v>
       </c>
-      <c r="Q16" s="0" t="n">
+      <c r="Q16" s="7" t="n">
         <v>220</v>
       </c>
-      <c r="R16" s="0" t="n">
+      <c r="R16" s="7" t="n">
         <f aca="false">SUM(P16:Q16)</f>
         <v>359</v>
       </c>
-      <c r="S16" s="0" t="n">
+      <c r="S16" s="7" t="n">
         <v>422</v>
       </c>
-      <c r="T16" s="0" t="n">
+      <c r="T16" s="7" t="n">
         <f aca="false">SUM(P16:R16)</f>
         <v>718</v>
       </c>
-      <c r="U16" s="1" t="n">
+      <c r="U16" s="6" t="n">
         <f aca="false">SUM(P16:Q16)+5*S16</f>
         <v>2469</v>
       </c>

</xml_diff>